<commit_message>
mac debug. settings dhcp or static IP
</commit_message>
<xml_diff>
--- a/firmware/chanels/regmap.xlsx
+++ b/firmware/chanels/regmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Radio\Jobe\LED_Driver_ETH\firmware\chanels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD11DE5E-1AA1-4830-893A-2583E17EDB83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC7178E-4F64-4ACD-919A-19B9DC42B76C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="12">
   <si>
     <t>htim3.Instance-&gt;CCR1</t>
   </si>
@@ -54,10 +54,13 @@
     <t>U_current 3</t>
   </si>
   <si>
-    <t>rx</t>
-  </si>
-  <si>
-    <t>tx</t>
+    <t>rx(что передает контроллер каналов)</t>
+  </si>
+  <si>
+    <t>tx(что контроллер принимает)</t>
+  </si>
+  <si>
+    <t>биты</t>
   </si>
 </sst>
 </file>
@@ -418,18 +421,23 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="29.21875" customWidth="1"/>
     <col min="6" max="6" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>

</xml_diff>